<commit_message>
final changes 17th march 2022
</commit_message>
<xml_diff>
--- a/FedExApplication/bin/TestFiles/FedExShipments.xlsx
+++ b/FedExApplication/bin/TestFiles/FedExShipments.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="391" uniqueCount="124">
   <si>
     <t>Nothing Bundt Cakes</t>
   </si>
@@ -311,6 +311,81 @@
   </si>
   <si>
     <t>320017993203</t>
+  </si>
+  <si>
+    <t>320018063820</t>
+  </si>
+  <si>
+    <t>320018063831</t>
+  </si>
+  <si>
+    <t>320018063864</t>
+  </si>
+  <si>
+    <t>320018063886</t>
+  </si>
+  <si>
+    <t>320018063923</t>
+  </si>
+  <si>
+    <t>320018063945</t>
+  </si>
+  <si>
+    <t>320018063978</t>
+  </si>
+  <si>
+    <t>320018063990</t>
+  </si>
+  <si>
+    <t>320018064025</t>
+  </si>
+  <si>
+    <t>320018064047</t>
+  </si>
+  <si>
+    <t>320018064080</t>
+  </si>
+  <si>
+    <t>320018064106</t>
+  </si>
+  <si>
+    <t>320018064139</t>
+  </si>
+  <si>
+    <t>320018064150</t>
+  </si>
+  <si>
+    <t>320018064183</t>
+  </si>
+  <si>
+    <t>320018064209</t>
+  </si>
+  <si>
+    <t>320018064242</t>
+  </si>
+  <si>
+    <t>320018064264</t>
+  </si>
+  <si>
+    <t>320018064297</t>
+  </si>
+  <si>
+    <t>320018064312</t>
+  </si>
+  <si>
+    <t>320018064345</t>
+  </si>
+  <si>
+    <t>320018064356</t>
+  </si>
+  <si>
+    <t>$248.51</t>
+  </si>
+  <si>
+    <t>320018064367</t>
+  </si>
+  <si>
+    <t>320018064378</t>
   </si>
 </sst>
 </file>
@@ -867,7 +942,7 @@
         <v>1</v>
       </c>
       <c r="P2" t="s">
-        <v>57</v>
+        <v>99</v>
       </c>
       <c r="Q2" t="s">
         <v>55</v>
@@ -920,7 +995,7 @@
         <v>3</v>
       </c>
       <c r="P3" t="s">
-        <v>59</v>
+        <v>100</v>
       </c>
       <c r="Q3" t="s">
         <v>58</v>
@@ -973,7 +1048,7 @@
         <v>2</v>
       </c>
       <c r="P4" t="s">
-        <v>61</v>
+        <v>101</v>
       </c>
       <c r="Q4" t="s">
         <v>60</v>
@@ -1026,7 +1101,7 @@
         <v>4</v>
       </c>
       <c r="P5" t="s">
-        <v>63</v>
+        <v>102</v>
       </c>
       <c r="Q5" t="s">
         <v>62</v>
@@ -1079,7 +1154,7 @@
         <v>2</v>
       </c>
       <c r="P6" t="s">
-        <v>65</v>
+        <v>103</v>
       </c>
       <c r="Q6" t="s">
         <v>64</v>
@@ -1132,7 +1207,7 @@
         <v>3</v>
       </c>
       <c r="P7" t="s">
-        <v>67</v>
+        <v>104</v>
       </c>
       <c r="Q7" t="s">
         <v>66</v>
@@ -1185,7 +1260,7 @@
         <v>2</v>
       </c>
       <c r="P8" t="s">
-        <v>68</v>
+        <v>105</v>
       </c>
       <c r="Q8" t="s">
         <v>55</v>
@@ -1238,7 +1313,7 @@
         <v>3</v>
       </c>
       <c r="P9" t="s">
-        <v>70</v>
+        <v>106</v>
       </c>
       <c r="Q9" t="s">
         <v>69</v>
@@ -1291,7 +1366,7 @@
         <v>2</v>
       </c>
       <c r="P10" t="s">
-        <v>71</v>
+        <v>107</v>
       </c>
       <c r="Q10" t="s">
         <v>58</v>
@@ -1344,7 +1419,7 @@
         <v>4</v>
       </c>
       <c r="P11" t="s">
-        <v>73</v>
+        <v>108</v>
       </c>
       <c r="Q11" t="s">
         <v>72</v>
@@ -1397,7 +1472,7 @@
         <v>2</v>
       </c>
       <c r="P12" t="s">
-        <v>75</v>
+        <v>109</v>
       </c>
       <c r="Q12" t="s">
         <v>74</v>
@@ -1450,7 +1525,7 @@
         <v>3</v>
       </c>
       <c r="P13" t="s">
-        <v>77</v>
+        <v>110</v>
       </c>
       <c r="Q13" t="s">
         <v>76</v>
@@ -1503,7 +1578,7 @@
         <v>2</v>
       </c>
       <c r="P14" t="s">
-        <v>79</v>
+        <v>111</v>
       </c>
       <c r="Q14" t="s">
         <v>78</v>
@@ -1556,7 +1631,7 @@
         <v>3</v>
       </c>
       <c r="P15" t="s">
-        <v>81</v>
+        <v>112</v>
       </c>
       <c r="Q15" t="s">
         <v>80</v>
@@ -1609,7 +1684,7 @@
         <v>2</v>
       </c>
       <c r="P16" t="s">
-        <v>82</v>
+        <v>113</v>
       </c>
       <c r="Q16" t="s">
         <v>60</v>
@@ -1662,7 +1737,7 @@
         <v>4</v>
       </c>
       <c r="P17" t="s">
-        <v>84</v>
+        <v>114</v>
       </c>
       <c r="Q17" t="s">
         <v>83</v>
@@ -1715,7 +1790,7 @@
         <v>2</v>
       </c>
       <c r="P18" t="s">
-        <v>85</v>
+        <v>115</v>
       </c>
       <c r="Q18" t="s">
         <v>62</v>
@@ -1768,7 +1843,7 @@
         <v>3</v>
       </c>
       <c r="P19" t="s">
-        <v>87</v>
+        <v>116</v>
       </c>
       <c r="Q19" t="s">
         <v>86</v>
@@ -1821,7 +1896,7 @@
         <v>2</v>
       </c>
       <c r="P20" t="s">
-        <v>89</v>
+        <v>117</v>
       </c>
       <c r="Q20" t="s">
         <v>88</v>
@@ -1874,7 +1949,7 @@
         <v>3</v>
       </c>
       <c r="P21" t="s">
-        <v>91</v>
+        <v>118</v>
       </c>
       <c r="Q21" t="s">
         <v>90</v>
@@ -1927,7 +2002,7 @@
         <v>2</v>
       </c>
       <c r="P22" t="s">
-        <v>93</v>
+        <v>119</v>
       </c>
       <c r="Q22" t="s">
         <v>92</v>
@@ -1980,7 +2055,7 @@
         <v>1</v>
       </c>
       <c r="P23" t="s">
-        <v>95</v>
+        <v>120</v>
       </c>
       <c r="Q23" t="s">
         <v>94</v>
@@ -2033,10 +2108,10 @@
         <v>1</v>
       </c>
       <c r="P24" t="s">
-        <v>97</v>
+        <v>122</v>
       </c>
       <c r="Q24" t="s">
-        <v>96</v>
+        <v>121</v>
       </c>
       <c r="R24" t="s">
         <v>52</v>
@@ -2086,7 +2161,7 @@
         <v>1</v>
       </c>
       <c r="P25" t="s">
-        <v>98</v>
+        <v>123</v>
       </c>
       <c r="Q25" t="s">
         <v>74</v>

</xml_diff>